<commit_message>
met thiet a cho
</commit_message>
<xml_diff>
--- a/Lab 01 - Nhóm 03 .xlsx
+++ b/Lab 01 - Nhóm 03 .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nguyen Nhat Hao\Downloads\CÔNG NGHỆ PHẦN MỀM NÂNG CAO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nguyen Nhat Hao\OneDrive\Desktop\CNPMNC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0CEF5C-4123-4B5A-983A-08FD6358780E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06AAB12-0ADE-4520-A690-9910F89A101F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="798" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="798" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Information" sheetId="7" r:id="rId1"/>
@@ -266,7 +266,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -313,6 +313,17 @@
     </font>
     <font>
       <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -535,7 +546,6 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -573,15 +583,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -606,11 +607,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,248 +1050,248 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="B27" s="12"/>
+      <c r="D27" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1309,14 +1320,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -1402,7 +1413,7 @@
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="9">
@@ -1411,13 +1422,13 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E8" s="15"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="15"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E10" s="15"/>
+      <c r="E10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1431,11 +1442,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1443,19 +1454,22 @@
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="5"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1465,377 +1479,468 @@
       <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18" t="s">
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
         <v>1</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="C6" s="29">
+        <v>3</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
         <v>2</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="14">
-        <v>3</v>
-      </c>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
-        <v>3</v>
-      </c>
-      <c r="B8" s="32" t="s">
+      <c r="C7" s="13">
+        <v>3</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+    </row>
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>3</v>
+      </c>
+      <c r="B8" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="C8" s="13">
+        <v>3</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+    </row>
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
         <v>4</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="C9" s="13">
+        <v>3</v>
+      </c>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
         <v>5</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+      <c r="C10" s="13">
+        <v>3</v>
+      </c>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
         <v>6</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
         <v>7</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
+      <c r="C12" s="22">
+        <v>3</v>
+      </c>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
         <v>8</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="29"/>
-    </row>
-    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="C13" s="28"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
         <v>9</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
         <v>10</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="C15" s="13">
+        <v>3</v>
+      </c>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
         <v>11</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="C16" s="13">
+        <v>3</v>
+      </c>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
         <v>12</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
         <v>13</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="C18" s="13">
+        <v>3</v>
+      </c>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
         <v>14</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="C19" s="13">
+        <v>3</v>
+      </c>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+    </row>
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
         <v>15</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="22">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+    </row>
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
         <v>16</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="25"/>
-    </row>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="C21" s="24"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
         <v>17</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+    </row>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
         <v>18</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
+      <c r="C23" s="19">
+        <v>3</v>
+      </c>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
         <v>19</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="20"/>
-    </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
+      <c r="B24" s="20"/>
+      <c r="C24" s="19"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+    </row>
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="19">
         <v>20</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="25"/>
-    </row>
-    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
+      <c r="C25" s="24"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
         <v>21</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="20">
+      <c r="C26" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="19">
         <v>22</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
+      <c r="C27" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="19">
         <v>23</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="20">
+      <c r="C28" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
         <v>24</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="20">
+      <c r="C29" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="19">
         <v>25</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="20">
+      <c r="C30" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="19">
         <v>26</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="25"/>
-    </row>
-    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
+      <c r="C31" s="24"/>
+    </row>
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="19">
         <v>27</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
+      <c r="A33" s="19">
         <v>28</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="20">
+      <c r="A34" s="19">
         <v>29</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
+      <c r="A35" s="19">
         <v>30</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="20">
+      <c r="A36" s="19">
         <v>31</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="20">
+      <c r="A37" s="19">
         <v>32</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
+      <c r="A38" s="19">
         <v>33</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="27">
+      <c r="C38" s="26">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1849,733 +1954,720 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.28515625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="37" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="37"/>
+    <col min="1" max="1" width="15" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="33" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="38"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
+      <c r="B3" s="34"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="50" t="s">
+      <c r="I4" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="50" t="s">
+      <c r="J4" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35">
         <f>SUM(C7:C10)</f>
         <v>11</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="39">
+      <c r="A7" s="35">
         <v>1</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="40">
-        <v>3</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
+      <c r="C7" s="36">
+        <v>3</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="39">
+      <c r="A8" s="35">
         <v>2</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="43">
-        <v>3</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
+      <c r="C8" s="39">
+        <v>3</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="39">
-        <v>3</v>
-      </c>
-      <c r="B9" s="44" t="s">
+      <c r="A9" s="35">
+        <v>3</v>
+      </c>
+      <c r="B9" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="43">
-        <v>3</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
+      <c r="C9" s="39">
+        <v>3</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="39">
+      <c r="A10" s="35">
         <v>4</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="39">
         <v>2</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="39">
+      <c r="A11" s="35">
         <v>5</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="46">
-        <v>3</v>
-      </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
+      <c r="C11" s="42">
+        <v>3</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="39">
+      <c r="A12" s="35">
         <v>6</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="G16" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="50" t="s">
+      <c r="H16" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="50" t="s">
+      <c r="I16" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="50" t="s">
+      <c r="J16" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="39">
+      <c r="A19" s="35">
         <v>1</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="39">
+      <c r="A20" s="35">
         <v>2</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="39">
-        <v>3</v>
-      </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
+      <c r="A21" s="35">
+        <v>3</v>
+      </c>
+      <c r="B21" s="44"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="39">
+      <c r="A22" s="35">
         <v>4</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="39">
+      <c r="A23" s="35">
         <v>5</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="39">
+      <c r="A24" s="35">
         <v>6</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="39">
+      <c r="A25" s="35">
         <v>7</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="50" t="s">
+      <c r="E28" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="50" t="s">
+      <c r="F28" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="50" t="s">
+      <c r="G28" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="50" t="s">
+      <c r="H28" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="50" t="s">
+      <c r="I28" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="39"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39">
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35">
         <f>SUM(C31:C34)</f>
         <v>11</v>
       </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="39">
+      <c r="A31" s="35">
         <v>1</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="40">
-        <v>3</v>
-      </c>
-      <c r="D31" s="39"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
+      <c r="C31" s="36">
+        <v>3</v>
+      </c>
+      <c r="D31" s="35"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="39">
+      <c r="A32" s="35">
         <v>2</v>
       </c>
-      <c r="C32" s="43">
-        <v>3</v>
-      </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
+      <c r="C32" s="39">
+        <v>3</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="39">
-        <v>3</v>
-      </c>
-      <c r="B33" s="44" t="s">
+      <c r="A33" s="35">
+        <v>3</v>
+      </c>
+      <c r="B33" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="43">
-        <v>3</v>
-      </c>
-      <c r="D33" s="39"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
+      <c r="C33" s="39">
+        <v>3</v>
+      </c>
+      <c r="D33" s="35"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="39">
+      <c r="A34" s="35">
         <v>4</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="39">
         <v>2</v>
       </c>
-      <c r="D34" s="39"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="39">
+      <c r="A35" s="35">
         <v>5</v>
       </c>
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="46">
-        <v>3</v>
-      </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
+      <c r="C35" s="42">
+        <v>3</v>
+      </c>
+      <c r="D35" s="43"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="39">
+      <c r="A36" s="35">
         <v>6</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="50" t="s">
+      <c r="C40" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="50" t="s">
+      <c r="D40" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="50" t="s">
+      <c r="E40" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="50" t="s">
+      <c r="F40" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="50" t="s">
+      <c r="G40" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="50" t="s">
+      <c r="H40" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="I40" s="50" t="s">
+      <c r="I40" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="J40" s="50" t="s">
+      <c r="J40" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39">
+      <c r="A41" s="35"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35">
         <f>SUM(C43:C46)</f>
         <v>11</v>
       </c>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="54" t="s">
+      <c r="A42" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="54"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="39">
+      <c r="A43" s="35">
         <v>1</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="40">
-        <v>3</v>
-      </c>
-      <c r="D43" s="39"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="C43" s="36">
+        <v>3</v>
+      </c>
+      <c r="D43" s="35"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="39">
+      <c r="A44" s="35">
         <v>2</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="43">
-        <v>3</v>
-      </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
+      <c r="C44" s="39">
+        <v>3</v>
+      </c>
+      <c r="D44" s="35"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="39">
-        <v>3</v>
-      </c>
-      <c r="B45" s="44" t="s">
+      <c r="A45" s="35">
+        <v>3</v>
+      </c>
+      <c r="B45" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="43">
-        <v>3</v>
-      </c>
-      <c r="D45" s="39"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="C45" s="39">
+        <v>3</v>
+      </c>
+      <c r="D45" s="35"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" s="39">
+      <c r="A46" s="35">
         <v>4</v>
       </c>
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="39">
         <v>2</v>
       </c>
-      <c r="D46" s="39"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="39">
+      <c r="A47" s="35">
         <v>5</v>
       </c>
-      <c r="B47" s="48" t="s">
+      <c r="B47" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="46">
-        <v>3</v>
-      </c>
-      <c r="D47" s="47"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="C47" s="42">
+        <v>3</v>
+      </c>
+      <c r="D47" s="43"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A48" s="39">
+      <c r="A48" s="35">
         <v>6</v>
       </c>
-      <c r="B48" s="48" t="s">
+      <c r="B48" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="39">
+      <c r="C48" s="35">
         <v>2</v>
       </c>
-      <c r="D48" s="47"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A49" s="39">
+      <c r="A49" s="35">
         <v>7</v>
       </c>
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="39">
+      <c r="C49" s="35">
         <v>5</v>
       </c>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="39"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="39"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>